<commit_message>
2021.10.05 BH update for examples, Java
</commit_message>
<xml_diff>
--- a/java/topoCifTags.xlsx
+++ b/java/topoCifTags.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hansonr\git\TopoCif\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6AC0CF9-A208-43E9-818E-16F958A87E75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C92AED4-0051-4B48-9D6C-9FFCD1C218D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="64">
   <si>
     <t>topol_link_id</t>
   </si>
@@ -45,9 +45,6 @@
     <t>topol_link_node_id_2</t>
   </si>
   <si>
-    <t>topol_link_symop_1</t>
-  </si>
-  <si>
     <t>topol_link_translation_1</t>
   </si>
   <si>
@@ -60,9 +57,6 @@
     <t>topol_link_translation_1_z</t>
   </si>
   <si>
-    <t>topol_link_symop_2</t>
-  </si>
-  <si>
     <t>topol_link_translation_2</t>
   </si>
   <si>
@@ -108,12 +102,6 @@
     <t>topol_atom_translation_z</t>
   </si>
   <si>
-    <t>topol_atom_symop</t>
-  </si>
-  <si>
-    <t>topol_node_symop</t>
-  </si>
-  <si>
     <t>topol_atom_fract_x</t>
   </si>
   <si>
@@ -195,9 +183,6 @@
     <t>topol_node_net_id</t>
   </si>
   <si>
-    <t>topol_node_chemical_formula_sum</t>
-  </si>
-  <si>
     <t>topol_net_id</t>
   </si>
   <si>
@@ -228,13 +213,16 @@
     <t>topol_net_special_details</t>
   </si>
   <si>
-    <t>topol_link_atom_label_1</t>
-  </si>
-  <si>
-    <t>topol_link_atom_label_2</t>
-  </si>
-  <si>
-    <t>topol_node_atom_label</t>
+    <t>topol_link_symop_id_1</t>
+  </si>
+  <si>
+    <t>topol_link_symop_id_2</t>
+  </si>
+  <si>
+    <t>topol_atom_symop_id</t>
+  </si>
+  <si>
+    <t>topol_node_symop_id</t>
   </si>
 </sst>
 </file>
@@ -1075,9 +1063,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E64"/>
+  <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
@@ -1089,19 +1079,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.75">
@@ -1109,14 +1099,14 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D2" t="str">
         <f>"/*"&amp;B2&amp;"*/"&amp;"""_"&amp;C2&amp;""","</f>
         <v>/*0*/"_topol_net_id",</v>
       </c>
       <c r="E2" t="str">
-        <f>"private final static byte "&amp;C2&amp;" = " &amp;B2&amp;";"</f>
+        <f>"private final static byte "&amp;C2&amp;IF(ISBLANK(A2),"","_DEPRECATED")&amp;" = " &amp;B2&amp;";"</f>
         <v>private final static byte topol_net_id = 0;</v>
       </c>
     </row>
@@ -1125,14 +1115,14 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D3" t="str">
         <f>"/*"&amp;B3&amp;"*/"&amp;"""_"&amp;C3&amp;""","</f>
         <v>/*1*/"_topol_net_label",</v>
       </c>
       <c r="E3" t="str">
-        <f>"private final static byte "&amp;C3&amp;" = " &amp;B3&amp;";"</f>
+        <f t="shared" ref="E3:E63" si="0">"private final static byte "&amp;C3&amp;IF(ISBLANK(A3),"","_DEPRECATED")&amp;" = " &amp;B3&amp;";"</f>
         <v>private final static byte topol_net_label = 1;</v>
       </c>
     </row>
@@ -1141,14 +1131,14 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D4" t="str">
         <f>"/*"&amp;B4&amp;"*/"&amp;"""_"&amp;C4&amp;""","</f>
         <v>/*2*/"_topol_net_special_details",</v>
       </c>
       <c r="E4" t="str">
-        <f>"private final static byte "&amp;C4&amp;" = " &amp;B4&amp;";"</f>
+        <f t="shared" si="0"/>
         <v>private final static byte topol_net_special_details = 2;</v>
       </c>
     </row>
@@ -1160,11 +1150,11 @@
         <v>0</v>
       </c>
       <c r="D5" t="str">
-        <f t="shared" ref="D5:D63" si="0">"/*"&amp;B5&amp;"*/"&amp;"""_"&amp;C5&amp;""","</f>
+        <f t="shared" ref="D5:D57" si="1">"/*"&amp;B5&amp;"*/"&amp;"""_"&amp;C5&amp;""","</f>
         <v>/*3*/"_topol_link_id",</v>
       </c>
       <c r="E5" t="str">
-        <f t="shared" ref="E5:E63" si="1">"private final static byte "&amp;C5&amp;" = " &amp;B5&amp;";"</f>
+        <f t="shared" si="0"/>
         <v>private final static byte topol_link_id = 3;</v>
       </c>
     </row>
@@ -1176,11 +1166,11 @@
         <v>1</v>
       </c>
       <c r="D6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>/*4*/"_topol_link_net_id",</v>
       </c>
       <c r="E6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>private final static byte topol_link_net_id = 4;</v>
       </c>
     </row>
@@ -1192,11 +1182,11 @@
         <v>2</v>
       </c>
       <c r="D7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>/*5*/"_topol_link_node_id_1",</v>
       </c>
       <c r="E7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>private final static byte topol_link_node_id_1 = 5;</v>
       </c>
     </row>
@@ -1208,11 +1198,11 @@
         <v>3</v>
       </c>
       <c r="D8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>/*6*/"_topol_link_node_id_2",</v>
       </c>
       <c r="E8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>private final static byte topol_link_node_id_2 = 6;</v>
       </c>
     </row>
@@ -1221,15 +1211,15 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="D9" t="str">
-        <f t="shared" si="0"/>
-        <v>/*7*/"_topol_link_node_label_1",</v>
+        <f t="shared" si="1"/>
+        <v>/*7*/"_topol_link_symop_id_1",</v>
       </c>
       <c r="E9" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_link_node_label_1 = 7;</v>
+        <f t="shared" si="0"/>
+        <v>private final static byte topol_link_symop_id_1 = 7;</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.75">
@@ -1237,15 +1227,15 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="D10" t="str">
-        <f t="shared" si="0"/>
-        <v>/*8*/"_topol_link_node_label_2",</v>
+        <f t="shared" si="1"/>
+        <v>/*8*/"_topol_link_translation_1",</v>
       </c>
       <c r="E10" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_link_node_label_2 = 8;</v>
+        <f t="shared" si="0"/>
+        <v>private final static byte topol_link_translation_1 = 8;</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.75">
@@ -1253,15 +1243,15 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>65</v>
+        <v>5</v>
       </c>
       <c r="D11" t="str">
-        <f t="shared" si="0"/>
-        <v>/*9*/"_topol_link_atom_label_1",</v>
+        <f t="shared" si="1"/>
+        <v>/*9*/"_topol_link_translation_1_x",</v>
       </c>
       <c r="E11" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_link_atom_label_1 = 9;</v>
+        <f t="shared" si="0"/>
+        <v>private final static byte topol_link_translation_1_x = 9;</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.75">
@@ -1269,15 +1259,15 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="D12" t="str">
-        <f t="shared" si="0"/>
-        <v>/*10*/"_topol_link_atom_label_2",</v>
+        <f t="shared" si="1"/>
+        <v>/*10*/"_topol_link_translation_1_y",</v>
       </c>
       <c r="E12" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_link_atom_label_2 = 10;</v>
+        <f t="shared" si="0"/>
+        <v>private final static byte topol_link_translation_1_y = 10;</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.75">
@@ -1285,15 +1275,15 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D13" t="str">
-        <f t="shared" si="0"/>
-        <v>/*11*/"_topol_link_symop_1",</v>
+        <f t="shared" si="1"/>
+        <v>/*11*/"_topol_link_translation_1_z",</v>
       </c>
       <c r="E13" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_link_symop_1 = 11;</v>
+        <f t="shared" si="0"/>
+        <v>private final static byte topol_link_translation_1_z = 11;</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.75">
@@ -1301,15 +1291,15 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="D14" t="str">
-        <f t="shared" si="0"/>
-        <v>/*12*/"_topol_link_translation_1",</v>
+        <f t="shared" si="1"/>
+        <v>/*12*/"_topol_link_symop_id_2",</v>
       </c>
       <c r="E14" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_link_translation_1 = 12;</v>
+        <f t="shared" si="0"/>
+        <v>private final static byte topol_link_symop_id_2 = 12;</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.75">
@@ -1317,15 +1307,15 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D15" t="str">
-        <f t="shared" si="0"/>
-        <v>/*13*/"_topol_link_translation_1_x",</v>
+        <f t="shared" si="1"/>
+        <v>/*13*/"_topol_link_translation_2",</v>
       </c>
       <c r="E15" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_link_translation_1_x = 13;</v>
+        <f t="shared" si="0"/>
+        <v>private final static byte topol_link_translation_2 = 13;</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.75">
@@ -1333,15 +1323,15 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D16" t="str">
-        <f t="shared" si="0"/>
-        <v>/*14*/"_topol_link_translation_1_y",</v>
+        <f t="shared" si="1"/>
+        <v>/*14*/"_topol_link_translation_2_x",</v>
       </c>
       <c r="E16" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_link_translation_1_y = 14;</v>
+        <f t="shared" si="0"/>
+        <v>private final static byte topol_link_translation_2_x = 14;</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.75">
@@ -1349,15 +1339,15 @@
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D17" t="str">
-        <f t="shared" si="0"/>
-        <v>/*15*/"_topol_link_translation_1_z",</v>
+        <f t="shared" si="1"/>
+        <v>/*15*/"_topol_link_translation_2_y",</v>
       </c>
       <c r="E17" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_link_translation_1_z = 15;</v>
+        <f t="shared" si="0"/>
+        <v>private final static byte topol_link_translation_2_y = 15;</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.75">
@@ -1365,15 +1355,15 @@
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D18" t="str">
-        <f t="shared" si="0"/>
-        <v>/*16*/"_topol_link_symop_2",</v>
+        <f t="shared" si="1"/>
+        <v>/*16*/"_topol_link_translation_2_z",</v>
       </c>
       <c r="E18" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_link_symop_2 = 16;</v>
+        <f t="shared" si="0"/>
+        <v>private final static byte topol_link_translation_2_z = 16;</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.75">
@@ -1381,15 +1371,15 @@
         <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="D19" t="str">
-        <f t="shared" si="0"/>
-        <v>/*17*/"_topol_link_translation_2",</v>
+        <f t="shared" si="1"/>
+        <v>/*17*/"_topol_link_distance",</v>
       </c>
       <c r="E19" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_link_translation_2 = 17;</v>
+        <f t="shared" si="0"/>
+        <v>private final static byte topol_link_distance = 17;</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.75">
@@ -1397,15 +1387,15 @@
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="D20" t="str">
-        <f t="shared" si="0"/>
-        <v>/*18*/"_topol_link_translation_2_x",</v>
+        <f t="shared" si="1"/>
+        <v>/*18*/"_topol_link_type",</v>
       </c>
       <c r="E20" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_link_translation_2_x = 18;</v>
+        <f t="shared" si="0"/>
+        <v>private final static byte topol_link_type = 18;</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.75">
@@ -1413,15 +1403,15 @@
         <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="D21" t="str">
-        <f t="shared" si="0"/>
-        <v>/*19*/"_topol_link_translation_2_y",</v>
+        <f t="shared" si="1"/>
+        <v>/*19*/"_topol_link_multiplicity",</v>
       </c>
       <c r="E21" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_link_translation_2_y = 19;</v>
+        <f t="shared" si="0"/>
+        <v>private final static byte topol_link_multiplicity = 19;</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.75">
@@ -1429,15 +1419,15 @@
         <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="D22" t="str">
-        <f t="shared" si="0"/>
-        <v>/*20*/"_topol_link_translation_2_z",</v>
+        <f t="shared" si="1"/>
+        <v>/*20*/"_topol_link_voronoi_solidangle",</v>
       </c>
       <c r="E22" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_link_translation_2_z = 20;</v>
+        <f t="shared" si="0"/>
+        <v>private final static byte topol_link_voronoi_solidangle = 20;</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.75">
@@ -1445,15 +1435,15 @@
         <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="D23" t="str">
-        <f t="shared" si="0"/>
-        <v>/*21*/"_topol_link_distance",</v>
+        <f t="shared" si="1"/>
+        <v>/*21*/"_topol_link_order",</v>
       </c>
       <c r="E23" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_link_distance = 21;</v>
+        <f t="shared" si="0"/>
+        <v>private final static byte topol_link_order = 21;</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.75">
@@ -1461,15 +1451,15 @@
         <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="D24" t="str">
-        <f t="shared" si="0"/>
-        <v>/*22*/"_topol_link_type",</v>
+        <f t="shared" si="1"/>
+        <v>/*22*/"_topol_node_id",</v>
       </c>
       <c r="E24" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_link_type = 22;</v>
+        <f t="shared" si="0"/>
+        <v>private final static byte topol_node_id = 22;</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.75">
@@ -1477,15 +1467,15 @@
         <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="D25" t="str">
-        <f t="shared" si="0"/>
-        <v>/*23*/"_topol_link_multiplicity",</v>
+        <f t="shared" si="1"/>
+        <v>/*23*/"_topol_node_net_id",</v>
       </c>
       <c r="E25" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_link_multiplicity = 23;</v>
+        <f t="shared" si="0"/>
+        <v>private final static byte topol_node_net_id = 23;</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.75">
@@ -1496,12 +1486,12 @@
         <v>45</v>
       </c>
       <c r="D26" t="str">
-        <f t="shared" si="0"/>
-        <v>/*24*/"_topol_link_voronoi_solidangle",</v>
+        <f t="shared" si="1"/>
+        <v>/*24*/"_topol_node_label",</v>
       </c>
       <c r="E26" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_link_voronoi_solidangle = 24;</v>
+        <f t="shared" si="0"/>
+        <v>private final static byte topol_node_label = 24;</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.75">
@@ -1509,15 +1499,15 @@
         <v>25</v>
       </c>
       <c r="C27" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="D27" t="str">
-        <f t="shared" si="0"/>
-        <v>/*25*/"_topol_link_order",</v>
+        <f t="shared" si="1"/>
+        <v>/*25*/"_topol_node_symop_id",</v>
       </c>
       <c r="E27" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_link_order = 25;</v>
+        <f t="shared" si="0"/>
+        <v>private final static byte topol_node_symop_id = 25;</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.75">
@@ -1528,12 +1518,12 @@
         <v>14</v>
       </c>
       <c r="D28" t="str">
-        <f t="shared" si="0"/>
-        <v>/*26*/"_topol_node_id",</v>
+        <f t="shared" si="1"/>
+        <v>/*26*/"_topol_node_translation",</v>
       </c>
       <c r="E28" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_node_id = 26;</v>
+        <f t="shared" si="0"/>
+        <v>private final static byte topol_node_translation = 26;</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.75">
@@ -1541,15 +1531,15 @@
         <v>27</v>
       </c>
       <c r="C29" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="D29" t="str">
-        <f t="shared" si="0"/>
-        <v>/*27*/"_topol_node_net_id",</v>
+        <f t="shared" si="1"/>
+        <v>/*27*/"_topol_node_translation_x",</v>
       </c>
       <c r="E29" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_node_net_id = 27;</v>
+        <f t="shared" si="0"/>
+        <v>private final static byte topol_node_translation_x = 27;</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.75">
@@ -1557,15 +1547,15 @@
         <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="D30" t="str">
-        <f t="shared" si="0"/>
-        <v>/*28*/"_topol_node_label",</v>
+        <f t="shared" si="1"/>
+        <v>/*28*/"_topol_node_translation_y",</v>
       </c>
       <c r="E30" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_node_label = 28;</v>
+        <f t="shared" si="0"/>
+        <v>private final static byte topol_node_translation_y = 28;</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.75">
@@ -1573,15 +1563,15 @@
         <v>29</v>
       </c>
       <c r="C31" t="s">
-        <v>67</v>
+        <v>17</v>
       </c>
       <c r="D31" t="str">
-        <f t="shared" si="0"/>
-        <v>/*29*/"_topol_node_atom_label",</v>
+        <f t="shared" si="1"/>
+        <v>/*29*/"_topol_node_translation_z",</v>
       </c>
       <c r="E31" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_node_atom_label = 29;</v>
+        <f t="shared" si="0"/>
+        <v>private final static byte topol_node_translation_z = 29;</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.75">
@@ -1589,50 +1579,50 @@
         <v>30</v>
       </c>
       <c r="C32" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="D32" t="str">
-        <f t="shared" si="0"/>
-        <v>/*30*/"_topol_node_symop",</v>
+        <f t="shared" si="1"/>
+        <v>/*30*/"_topol_node_fract_x",</v>
       </c>
       <c r="E32" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_node_symop = 30;</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.75">
+        <f t="shared" si="0"/>
+        <v>private final static byte topol_node_fract_x = 30;</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.75">
       <c r="B33">
         <v>31</v>
       </c>
       <c r="C33" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="D33" t="str">
-        <f t="shared" si="0"/>
-        <v>/*31*/"_topol_node_translation",</v>
+        <f t="shared" si="1"/>
+        <v>/*31*/"_topol_node_fract_y",</v>
       </c>
       <c r="E33" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_node_translation = 31;</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.75">
+        <f t="shared" si="0"/>
+        <v>private final static byte topol_node_fract_y = 31;</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.75">
       <c r="B34">
         <v>32</v>
       </c>
       <c r="C34" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="D34" t="str">
-        <f t="shared" si="0"/>
-        <v>/*32*/"_topol_node_translation_x",</v>
+        <f t="shared" si="1"/>
+        <v>/*32*/"_topol_node_fract_z",</v>
       </c>
       <c r="E34" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_node_translation_x = 32;</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.75">
+        <f t="shared" si="0"/>
+        <v>private final static byte topol_node_fract_z = 32;</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.75">
       <c r="B35">
         <v>33</v>
       </c>
@@ -1640,95 +1630,95 @@
         <v>18</v>
       </c>
       <c r="D35" t="str">
-        <f t="shared" si="0"/>
-        <v>/*33*/"_topol_node_translation_y",</v>
+        <f t="shared" si="1"/>
+        <v>/*33*/"_topol_atom_id",</v>
       </c>
       <c r="E35" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_node_translation_y = 33;</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.75">
+        <f t="shared" si="0"/>
+        <v>private final static byte topol_atom_id = 33;</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.75">
       <c r="B36">
         <v>34</v>
       </c>
       <c r="C36" t="s">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="D36" t="str">
-        <f t="shared" si="0"/>
-        <v>/*34*/"_topol_node_translation_z",</v>
+        <f t="shared" si="1"/>
+        <v>/*34*/"_topol_atom_atom_label",</v>
       </c>
       <c r="E36" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_node_translation_z = 34;</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.75">
+        <f t="shared" si="0"/>
+        <v>private final static byte topol_atom_atom_label = 34;</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.75">
       <c r="B37">
         <v>35</v>
       </c>
       <c r="C37" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="D37" t="str">
-        <f t="shared" si="0"/>
-        <v>/*35*/"_topol_node_fract_x",</v>
+        <f t="shared" si="1"/>
+        <v>/*35*/"_topol_atom_node_id",</v>
       </c>
       <c r="E37" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_node_fract_x = 35;</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.75">
+        <f t="shared" si="0"/>
+        <v>private final static byte topol_atom_node_id = 35;</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.75">
       <c r="B38">
         <v>36</v>
       </c>
       <c r="C38" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="D38" t="str">
-        <f t="shared" si="0"/>
-        <v>/*36*/"_topol_node_fract_y",</v>
+        <f t="shared" si="1"/>
+        <v>/*36*/"_topol_atom_link_id",</v>
       </c>
       <c r="E38" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_node_fract_y = 36;</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.75">
+        <f t="shared" si="0"/>
+        <v>private final static byte topol_atom_link_id = 36;</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.75">
       <c r="B39">
         <v>37</v>
       </c>
       <c r="C39" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="D39" t="str">
-        <f t="shared" si="0"/>
-        <v>/*37*/"_topol_node_fract_z",</v>
+        <f t="shared" si="1"/>
+        <v>/*37*/"_topol_atom_symop_id",</v>
       </c>
       <c r="E39" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_node_fract_z = 37;</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.75">
+        <f t="shared" si="0"/>
+        <v>private final static byte topol_atom_symop_id = 37;</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.75">
       <c r="B40">
         <v>38</v>
       </c>
       <c r="C40" t="s">
-        <v>54</v>
+        <v>19</v>
       </c>
       <c r="D40" t="str">
-        <f t="shared" si="0"/>
-        <v>/*38*/"_topol_node_chemical_formula_sum",</v>
+        <f t="shared" si="1"/>
+        <v>/*38*/"_topol_atom_translation",</v>
       </c>
       <c r="E40" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_node_chemical_formula_sum = 38;</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.75">
+        <f t="shared" si="0"/>
+        <v>private final static byte topol_atom_translation = 38;</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.75">
       <c r="B41">
         <v>39</v>
       </c>
@@ -1736,399 +1726,336 @@
         <v>20</v>
       </c>
       <c r="D41" t="str">
-        <f t="shared" si="0"/>
-        <v>/*39*/"_topol_atom_id",</v>
+        <f t="shared" si="1"/>
+        <v>/*39*/"_topol_atom_translation_x",</v>
       </c>
       <c r="E41" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_atom_id = 39;</v>
-      </c>
-    </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.75">
+        <f t="shared" si="0"/>
+        <v>private final static byte topol_atom_translation_x = 39;</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.75">
       <c r="B42">
         <v>40</v>
       </c>
       <c r="C42" t="s">
-        <v>63</v>
+        <v>21</v>
       </c>
       <c r="D42" t="str">
-        <f t="shared" si="0"/>
-        <v>/*40*/"_topol_atom_atom_label",</v>
+        <f t="shared" si="1"/>
+        <v>/*40*/"_topol_atom_translation_y",</v>
       </c>
       <c r="E42" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_atom_atom_label = 40;</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.75">
+        <f t="shared" si="0"/>
+        <v>private final static byte topol_atom_translation_y = 40;</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.75">
       <c r="B43">
         <v>41</v>
       </c>
       <c r="C43" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D43" t="str">
-        <f t="shared" si="0"/>
-        <v>/*41*/"_topol_atom_node_id",</v>
+        <f t="shared" si="1"/>
+        <v>/*41*/"_topol_atom_translation_z",</v>
       </c>
       <c r="E43" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_atom_node_id = 41;</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.75">
+        <f t="shared" si="0"/>
+        <v>private final static byte topol_atom_translation_z = 41;</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.75">
       <c r="B44">
         <v>42</v>
       </c>
       <c r="C44" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D44" t="str">
-        <f t="shared" si="0"/>
-        <v>/*42*/"_topol_atom_link_id",</v>
+        <f t="shared" si="1"/>
+        <v>/*42*/"_topol_atom_fract_x",</v>
       </c>
       <c r="E44" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_atom_link_id = 42;</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.75">
+        <f t="shared" si="0"/>
+        <v>private final static byte topol_atom_fract_x = 42;</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.75">
       <c r="B45">
         <v>43</v>
       </c>
       <c r="C45" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D45" t="str">
-        <f t="shared" si="0"/>
-        <v>/*43*/"_topol_atom_symop",</v>
+        <f t="shared" si="1"/>
+        <v>/*43*/"_topol_atom_fract_y",</v>
       </c>
       <c r="E45" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_atom_symop = 43;</v>
-      </c>
-    </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.75">
+        <f t="shared" si="0"/>
+        <v>private final static byte topol_atom_fract_y = 43;</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.75">
       <c r="B46">
         <v>44</v>
       </c>
       <c r="C46" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D46" t="str">
-        <f t="shared" si="0"/>
-        <v>/*44*/"_topol_atom_translation",</v>
+        <f t="shared" si="1"/>
+        <v>/*44*/"_topol_atom_fract_z",</v>
       </c>
       <c r="E46" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_atom_translation = 44;</v>
-      </c>
-    </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.75">
+        <f t="shared" si="0"/>
+        <v>private final static byte topol_atom_fract_z = 44;</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.75">
       <c r="B47">
         <v>45</v>
       </c>
       <c r="C47" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="D47" t="str">
-        <f t="shared" si="0"/>
-        <v>/*45*/"_topol_atom_translation_x",</v>
+        <f t="shared" si="1"/>
+        <v>/*45*/"_topol_atom_element_symbol",</v>
       </c>
       <c r="E47" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_atom_translation_x = 45;</v>
-      </c>
-    </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.75">
+        <f t="shared" si="0"/>
+        <v>private final static byte topol_atom_element_symbol = 45;</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A48" t="s">
+        <v>52</v>
+      </c>
       <c r="B48">
         <v>46</v>
       </c>
       <c r="C48" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D48" t="str">
-        <f t="shared" si="0"/>
-        <v>/*46*/"_topol_atom_translation_y",</v>
+        <f t="shared" si="1"/>
+        <v>/*46*/"_topol_link_site_symmetry_symop_1",</v>
       </c>
       <c r="E48" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_atom_translation_y = 46;</v>
+        <f t="shared" si="0"/>
+        <v>private final static byte topol_link_site_symmetry_symop_1_DEPRECATED = 46;</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A49" t="s">
+        <v>52</v>
+      </c>
       <c r="B49">
         <v>47</v>
       </c>
       <c r="C49" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="D49" t="str">
-        <f t="shared" si="0"/>
-        <v>/*47*/"_topol_atom_translation_z",</v>
+        <f t="shared" si="1"/>
+        <v>/*47*/"_topol_link_site_symmetry_translation_1_x",</v>
       </c>
       <c r="E49" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_atom_translation_z = 47;</v>
+        <f t="shared" si="0"/>
+        <v>private final static byte topol_link_site_symmetry_translation_1_x_DEPRECATED = 47;</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A50" t="s">
+        <v>52</v>
+      </c>
       <c r="B50">
         <v>48</v>
       </c>
       <c r="C50" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D50" t="str">
-        <f t="shared" si="0"/>
-        <v>/*48*/"_topol_atom_fract_x",</v>
+        <f t="shared" si="1"/>
+        <v>/*48*/"_topol_link_site_symmetry_translation_1_y",</v>
       </c>
       <c r="E50" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_atom_fract_x = 48;</v>
+        <f t="shared" si="0"/>
+        <v>private final static byte topol_link_site_symmetry_translation_1_y_DEPRECATED = 48;</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A51" t="s">
+        <v>52</v>
+      </c>
       <c r="B51">
         <v>49</v>
       </c>
       <c r="C51" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D51" t="str">
-        <f t="shared" si="0"/>
-        <v>/*49*/"_topol_atom_fract_y",</v>
+        <f t="shared" si="1"/>
+        <v>/*49*/"_topol_link_site_symmetry_translation_1_z",</v>
       </c>
       <c r="E51" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_atom_fract_y = 49;</v>
+        <f t="shared" si="0"/>
+        <v>private final static byte topol_link_site_symmetry_translation_1_z_DEPRECATED = 49;</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A52" t="s">
+        <v>52</v>
+      </c>
       <c r="B52">
         <v>50</v>
       </c>
       <c r="C52" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="D52" t="str">
-        <f t="shared" si="0"/>
-        <v>/*50*/"_topol_atom_fract_z",</v>
+        <f t="shared" si="1"/>
+        <v>/*50*/"_topol_link_site_symmetry_symop_2",</v>
       </c>
       <c r="E52" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_atom_fract_z = 50;</v>
+        <f t="shared" si="0"/>
+        <v>private final static byte topol_link_site_symmetry_symop_2_DEPRECATED = 50;</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A53" t="s">
+        <v>52</v>
+      </c>
       <c r="B53">
         <v>51</v>
       </c>
       <c r="C53" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="D53" t="str">
-        <f t="shared" si="0"/>
-        <v>/*51*/"_topol_atom_element_symbol",</v>
+        <f t="shared" si="1"/>
+        <v>/*51*/"_topol_link_site_symmetry_translation_2_x",</v>
       </c>
       <c r="E53" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_atom_element_symbol = 51;</v>
+        <f t="shared" si="0"/>
+        <v>private final static byte topol_link_site_symmetry_translation_2_x_DEPRECATED = 51;</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A54" t="s">
+        <v>52</v>
+      </c>
       <c r="B54">
         <v>52</v>
       </c>
       <c r="C54" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D54" t="str">
-        <f t="shared" si="0"/>
-        <v>/*52*/"_topol_link_site_symmetry_symop_1",</v>
+        <f t="shared" si="1"/>
+        <v>/*52*/"_topol_link_site_symmetry_translation_2_y",</v>
       </c>
       <c r="E54" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_link_site_symmetry_symop_1 = 52;</v>
+        <f t="shared" si="0"/>
+        <v>private final static byte topol_link_site_symmetry_translation_2_y_DEPRECATED = 52;</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A55" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B55">
         <v>53</v>
       </c>
       <c r="C55" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D55" t="str">
-        <f t="shared" si="0"/>
-        <v>/*53*/"_topol_link_site_symmetry_translation_1_x",</v>
+        <f t="shared" si="1"/>
+        <v>/*53*/"_topol_link_site_symmetry_translation_2_z",</v>
       </c>
       <c r="E55" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_link_site_symmetry_translation_1_x = 53;</v>
+        <f t="shared" si="0"/>
+        <v>private final static byte topol_link_site_symmetry_translation_2_z_DEPRECATED = 53;</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A56" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B56">
         <v>54</v>
       </c>
       <c r="C56" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="D56" t="str">
-        <f t="shared" si="0"/>
-        <v>/*54*/"_topol_link_site_symmetry_translation_1_y",</v>
+        <f t="shared" si="1"/>
+        <v>/*54*/"_topol_link_site_symmetry_translation_1",</v>
       </c>
       <c r="E56" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_link_site_symmetry_translation_1_y = 54;</v>
+        <f t="shared" si="0"/>
+        <v>private final static byte topol_link_site_symmetry_translation_1_DEPRECATED = 54;</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A57" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B57">
         <v>55</v>
       </c>
       <c r="C57" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D57" t="str">
-        <f t="shared" si="0"/>
-        <v>/*55*/"_topol_link_site_symmetry_translation_1_z",</v>
+        <f t="shared" si="1"/>
+        <v>/*55*/"_topol_link_site_symmetry_translation_2",</v>
       </c>
       <c r="E57" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_link_site_symmetry_translation_1_z = 55;</v>
+        <f t="shared" si="0"/>
+        <v>private final static byte topol_link_site_symmetry_translation_2_DEPRECATED = 55;</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A58" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B58">
         <v>56</v>
       </c>
       <c r="C58" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="D58" t="str">
-        <f t="shared" si="0"/>
-        <v>/*56*/"_topol_link_site_symmetry_symop_2",</v>
+        <f>"/*"&amp;B58&amp;"*/"&amp;"""_"&amp;C58&amp;""","</f>
+        <v>/*56*/"_topol_link_node_label_1",</v>
       </c>
       <c r="E58" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_link_site_symmetry_symop_2 = 56;</v>
+        <f t="shared" si="0"/>
+        <v>private final static byte topol_link_node_label_1_DEPRECATED = 56;</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A59" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B59">
         <v>57</v>
       </c>
       <c r="C59" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="D59" t="str">
-        <f t="shared" si="0"/>
-        <v>/*57*/"_topol_link_site_symmetry_translation_2_x",</v>
+        <f>"/*"&amp;B59&amp;"*/"&amp;"""_"&amp;C59&amp;""","</f>
+        <v>/*57*/"_topol_link_node_label_2",</v>
       </c>
       <c r="E59" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_link_site_symmetry_translation_2_x = 57;</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A60" t="s">
-        <v>57</v>
-      </c>
-      <c r="B60">
-        <v>58</v>
-      </c>
-      <c r="C60" t="s">
-        <v>41</v>
-      </c>
-      <c r="D60" t="str">
-        <f t="shared" si="0"/>
-        <v>/*58*/"_topol_link_site_symmetry_translation_2_y",</v>
-      </c>
-      <c r="E60" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_link_site_symmetry_translation_2_y = 58;</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A61" t="s">
-        <v>57</v>
-      </c>
-      <c r="B61">
-        <v>59</v>
-      </c>
-      <c r="C61" t="s">
-        <v>42</v>
-      </c>
-      <c r="D61" t="str">
-        <f t="shared" si="0"/>
-        <v>/*59*/"_topol_link_site_symmetry_translation_2_z",</v>
-      </c>
-      <c r="E61" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_link_site_symmetry_translation_2_z = 59;</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A62" t="s">
-        <v>57</v>
-      </c>
-      <c r="B62">
-        <v>60</v>
-      </c>
-      <c r="C62" t="s">
-        <v>46</v>
-      </c>
-      <c r="D62" t="str">
-        <f t="shared" si="0"/>
-        <v>/*60*/"_topol_link_site_symmetry_translation_1",</v>
-      </c>
-      <c r="E62" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_link_site_symmetry_translation_1 = 60;</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A63" t="s">
-        <v>57</v>
-      </c>
-      <c r="B63">
-        <v>61</v>
-      </c>
-      <c r="C63" t="s">
-        <v>47</v>
-      </c>
-      <c r="D63" t="str">
-        <f t="shared" si="0"/>
-        <v>/*61*/"_topol_link_site_symmetry_translation_2",</v>
-      </c>
-      <c r="E63" t="str">
-        <f t="shared" si="1"/>
-        <v>private final static byte topol_link_site_symmetry_translation_2 = 61;</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A64" t="s">
-        <v>57</v>
-      </c>
-      <c r="B64">
-        <v>62</v>
+        <f t="shared" si="0"/>
+        <v>private final static byte topol_link_node_label_2_DEPRECATED = 57;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>